<commit_message>
fehler der masken behoben
</commit_message>
<xml_diff>
--- a/Notes/Befehle/PICBefehle_Maske.xlsx
+++ b/Notes/Befehle/PICBefehle_Maske.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PIC-Simulator\Notes\Befehle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38115E3B-34A4-4125-8801-45432EE76F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68778867-0FD7-4918-BA2D-608F20BB5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EE50DCF6-8A61-4489-B845-A4C8EC7BC426}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE50DCF6-8A61-4489-B845-A4C8EC7BC426}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -251,21 +251,6 @@
     <t>Maske</t>
   </si>
   <si>
-    <t>0xf8</t>
-  </si>
-  <si>
-    <t>0xfc</t>
-  </si>
-  <si>
-    <t>0xfe</t>
-  </si>
-  <si>
-    <t>0xff</t>
-  </si>
-  <si>
-    <t>0xff8</t>
-  </si>
-  <si>
     <t>0xffff</t>
   </si>
   <si>
@@ -399,6 +384,21 @@
   </si>
   <si>
     <t>(); break;</t>
+  </si>
+  <si>
+    <t>0xff80</t>
+  </si>
+  <si>
+    <t>0xff00</t>
+  </si>
+  <si>
+    <t>0xfe00</t>
+  </si>
+  <si>
+    <t>0xfc00</t>
+  </si>
+  <si>
+    <t>0xf800</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2358C5C1-01DA-4041-924F-58ABF6B05BD1}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:J28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,7 @@
         <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
         <v>70</v>
@@ -789,10 +789,10 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -803,10 +803,10 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -817,10 +817,10 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -831,10 +831,10 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -845,25 +845,25 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -874,31 +874,31 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G11" t="str">
         <f>C23</f>
         <v>0x0b00</v>
       </c>
       <c r="H11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I11" t="str">
         <f>A23</f>
         <v>decfsz</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L11" t="str">
         <f>D23</f>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -906,34 +906,34 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" ref="G12:G34" si="0">C24</f>
+        <f t="shared" ref="G12:G28" si="0">C24</f>
         <v>0x0c00</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ref="I12:I28" si="1">A24</f>
         <v>rrf</v>
       </c>
       <c r="J12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ref="L12:L28" si="2">D24</f>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -944,31 +944,31 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>0x0d00</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
         <v>rlf</v>
       </c>
       <c r="J13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -979,31 +979,31 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>0x0e00</v>
       </c>
       <c r="H14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
         <v>swapf</v>
       </c>
       <c r="J14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1014,31 +1014,31 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>0x0f00</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
         <v>incfsz</v>
       </c>
       <c r="J15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1049,31 +1049,31 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>0x3800</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
         <v>iorlw</v>
       </c>
       <c r="J16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1084,31 +1084,31 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>0x3900</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
         <v>ANDLW</v>
       </c>
       <c r="J17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1119,31 +1119,31 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>0x3a00</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
         <v>xorlw</v>
       </c>
       <c r="J18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="2"/>
-        <v>0xff</v>
+        <v>0xff00</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1154,31 +1154,31 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>0x3c00</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
         <v>sublw</v>
       </c>
       <c r="J19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="2"/>
-        <v>0xfe</v>
+        <v>0xfe00</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1189,31 +1189,31 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>0x3e00</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
         <v>ADDLW</v>
       </c>
       <c r="J20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="2"/>
-        <v>0xfe</v>
+        <v>0xfe00</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1224,31 +1224,31 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>0x1000</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
         <v>bcf</v>
       </c>
       <c r="J21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1256,34 +1256,34 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>0x1400</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
         <v>BSF</v>
       </c>
       <c r="J22" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1294,31 +1294,31 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v>0x1800</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
         <v>BTFSC</v>
       </c>
       <c r="J23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1329,31 +1329,31 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>0x1c00</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
         <v>BTFSS</v>
       </c>
       <c r="J24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1364,31 +1364,31 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>0x3000</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
         <v>movlw</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1399,31 +1399,31 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>0x3400</v>
       </c>
       <c r="H26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
         <v>retlw</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="2"/>
-        <v>0xfc</v>
+        <v>0xfc00</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1434,31 +1434,31 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F27" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>0x2800</v>
       </c>
       <c r="H27" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
         <v>goto</v>
       </c>
       <c r="J27" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="2"/>
-        <v>0xf8</v>
+        <v>0xf800</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1469,31 +1469,31 @@
         <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>0x2000</v>
       </c>
       <c r="H28" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="1"/>
         <v>CALL</v>
       </c>
       <c r="J28" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="2"/>
-        <v>0xf8</v>
+        <v>0xf800</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1504,10 +1504,10 @@
         <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1518,10 +1518,10 @@
         <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1532,10 +1532,10 @@
         <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1546,10 +1546,10 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,10 +1560,10 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,10 +1574,10 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,10 +1588,10 @@
         <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,10 +1602,10 @@
         <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,10 +1616,10 @@
         <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,10 +1630,10 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,10 +1644,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,10 +1658,10 @@
         <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>